<commit_message>
elaborates change; formalises commodities and management practices
</commit_message>
<xml_diff>
--- a/classification-systems/nzlum/build/nzlum_v0.3.0.xlsx
+++ b/classification-systems/nzlum/build/nzlum_v0.3.0.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F95"/>
+  <dimension ref="A1:F96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -918,40 +918,40 @@
     <row r="26">
       <c r="A26" s="2" t="n"/>
       <c r="B26" s="2" t="n"/>
-      <c r="C26" s="2" t="inlineStr">
-        <is>
-          <t>2.2.0</t>
-        </is>
-      </c>
-      <c r="D26" s="2" t="inlineStr">
-        <is>
-          <t>Grazing modified pasture systems</t>
-        </is>
-      </c>
+      <c r="C26" s="2" t="n"/>
+      <c r="D26" s="2" t="n"/>
       <c r="E26" s="2" t="inlineStr">
         <is>
-          <t>2.2.1</t>
+          <t>2.1.5</t>
         </is>
       </c>
       <c r="F26" s="2" t="inlineStr">
         <is>
-          <t>Dairy</t>
+          <t>Permanent carbon forest</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n"/>
       <c r="B27" s="2" t="n"/>
-      <c r="C27" s="2" t="n"/>
-      <c r="D27" s="2" t="n"/>
+      <c r="C27" s="2" t="inlineStr">
+        <is>
+          <t>2.2.0</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>Grazing modified pasture systems</t>
+        </is>
+      </c>
       <c r="E27" s="2" t="inlineStr">
         <is>
-          <t>2.2.2</t>
+          <t>2.2.1</t>
         </is>
       </c>
       <c r="F27" s="2" t="inlineStr">
         <is>
-          <t>Intensive dry stock</t>
+          <t>Dairy</t>
         </is>
       </c>
     </row>
@@ -962,52 +962,52 @@
       <c r="D28" s="2" t="n"/>
       <c r="E28" s="2" t="inlineStr">
         <is>
-          <t>2.2.3</t>
+          <t>2.2.2</t>
         </is>
       </c>
       <c r="F28" s="2" t="inlineStr">
         <is>
-          <t>Extensive dry stock</t>
+          <t>Intensive dry stock</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n"/>
       <c r="B29" s="2" t="n"/>
-      <c r="C29" s="2" t="inlineStr">
-        <is>
-          <t>2.3.0</t>
-        </is>
-      </c>
-      <c r="D29" s="2" t="inlineStr">
-        <is>
-          <t>Short-rotation and seasonal cropping</t>
-        </is>
-      </c>
+      <c r="C29" s="2" t="n"/>
+      <c r="D29" s="2" t="n"/>
       <c r="E29" s="2" t="inlineStr">
         <is>
-          <t>2.3.1</t>
+          <t>2.2.3</t>
         </is>
       </c>
       <c r="F29" s="2" t="inlineStr">
         <is>
-          <t>Arable cropping</t>
+          <t>Extensive dry stock</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n"/>
       <c r="B30" s="2" t="n"/>
-      <c r="C30" s="2" t="n"/>
-      <c r="D30" s="2" t="n"/>
+      <c r="C30" s="2" t="inlineStr">
+        <is>
+          <t>2.3.0</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>Short-rotation and seasonal cropping</t>
+        </is>
+      </c>
       <c r="E30" s="2" t="inlineStr">
         <is>
-          <t>2.3.2</t>
+          <t>2.3.1</t>
         </is>
       </c>
       <c r="F30" s="2" t="inlineStr">
         <is>
-          <t>Arable and mixed livestock cropping</t>
+          <t>Arable cropping</t>
         </is>
       </c>
     </row>
@@ -1018,12 +1018,12 @@
       <c r="D31" s="2" t="n"/>
       <c r="E31" s="2" t="inlineStr">
         <is>
-          <t>2.3.3</t>
+          <t>2.3.2</t>
         </is>
       </c>
       <c r="F31" s="2" t="inlineStr">
         <is>
-          <t>Short-rotation horticulture</t>
+          <t>Arable and mixed livestock cropping</t>
         </is>
       </c>
     </row>
@@ -1034,52 +1034,52 @@
       <c r="D32" s="2" t="n"/>
       <c r="E32" s="2" t="inlineStr">
         <is>
-          <t>2.3.4</t>
+          <t>2.3.3</t>
         </is>
       </c>
       <c r="F32" s="2" t="inlineStr">
         <is>
-          <t>Seasonal flowers and bulbs, and turf farming</t>
+          <t>Short-rotation horticulture</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n"/>
       <c r="B33" s="2" t="n"/>
-      <c r="C33" s="2" t="inlineStr">
-        <is>
-          <t>2.4.0</t>
-        </is>
-      </c>
-      <c r="D33" s="2" t="inlineStr">
-        <is>
-          <t>Perennial horticulture</t>
-        </is>
-      </c>
+      <c r="C33" s="2" t="n"/>
+      <c r="D33" s="2" t="n"/>
       <c r="E33" s="2" t="inlineStr">
         <is>
-          <t>2.4.1</t>
+          <t>2.3.4</t>
         </is>
       </c>
       <c r="F33" s="2" t="inlineStr">
         <is>
-          <t>Tree crops</t>
+          <t>Seasonal flowers and bulbs, and turf farming</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n"/>
       <c r="B34" s="2" t="n"/>
-      <c r="C34" s="2" t="n"/>
-      <c r="D34" s="2" t="n"/>
+      <c r="C34" s="2" t="inlineStr">
+        <is>
+          <t>2.4.0</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>Perennial horticulture</t>
+        </is>
+      </c>
       <c r="E34" s="2" t="inlineStr">
         <is>
-          <t>2.4.2</t>
+          <t>2.4.1</t>
         </is>
       </c>
       <c r="F34" s="2" t="inlineStr">
         <is>
-          <t>Vine fruits</t>
+          <t>Tree crops</t>
         </is>
       </c>
     </row>
@@ -1090,92 +1090,92 @@
       <c r="D35" s="2" t="n"/>
       <c r="E35" s="2" t="inlineStr">
         <is>
-          <t>2.4.3</t>
+          <t>2.4.2</t>
         </is>
       </c>
       <c r="F35" s="2" t="inlineStr">
         <is>
-          <t>Other perennial horticulture</t>
+          <t>Vine fruits</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n"/>
       <c r="B36" s="2" t="n"/>
-      <c r="C36" s="2" t="inlineStr">
-        <is>
-          <t>2.5.0</t>
-        </is>
-      </c>
-      <c r="D36" s="2" t="inlineStr">
-        <is>
-          <t>Intensive horticulture</t>
-        </is>
-      </c>
+      <c r="C36" s="2" t="n"/>
+      <c r="D36" s="2" t="n"/>
       <c r="E36" s="2" t="inlineStr">
         <is>
-          <t>2.5.1</t>
+          <t>2.4.3</t>
         </is>
       </c>
       <c r="F36" s="2" t="inlineStr">
         <is>
-          <t>Production nurseries</t>
+          <t>Other perennial horticulture</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n"/>
       <c r="B37" s="2" t="n"/>
-      <c r="C37" s="2" t="n"/>
-      <c r="D37" s="2" t="n"/>
+      <c r="C37" s="2" t="inlineStr">
+        <is>
+          <t>2.5.0</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>Intensive horticulture</t>
+        </is>
+      </c>
       <c r="E37" s="2" t="inlineStr">
         <is>
-          <t>2.5.2</t>
+          <t>2.5.1</t>
         </is>
       </c>
       <c r="F37" s="2" t="inlineStr">
         <is>
-          <t>Glasshouses/shadehouses</t>
+          <t>Production nurseries</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n"/>
       <c r="B38" s="2" t="n"/>
-      <c r="C38" s="2" t="inlineStr">
-        <is>
-          <t>2.6.0</t>
-        </is>
-      </c>
-      <c r="D38" s="2" t="inlineStr">
-        <is>
-          <t>Intensive animal production</t>
-        </is>
-      </c>
+      <c r="C38" s="2" t="n"/>
+      <c r="D38" s="2" t="n"/>
       <c r="E38" s="2" t="inlineStr">
         <is>
-          <t>2.6.1</t>
+          <t>2.5.2</t>
         </is>
       </c>
       <c r="F38" s="2" t="inlineStr">
         <is>
-          <t>Intensive animal containment</t>
+          <t>Glasshouses/shadehouses</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n"/>
       <c r="B39" s="2" t="n"/>
-      <c r="C39" s="2" t="n"/>
-      <c r="D39" s="2" t="n"/>
+      <c r="C39" s="2" t="inlineStr">
+        <is>
+          <t>2.6.0</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>Intensive animal production</t>
+        </is>
+      </c>
       <c r="E39" s="2" t="inlineStr">
         <is>
-          <t>2.6.2</t>
+          <t>2.6.1</t>
         </is>
       </c>
       <c r="F39" s="2" t="inlineStr">
         <is>
-          <t>Poultry farms</t>
+          <t>Intensive animal containment</t>
         </is>
       </c>
     </row>
@@ -1186,12 +1186,12 @@
       <c r="D40" s="2" t="n"/>
       <c r="E40" s="2" t="inlineStr">
         <is>
-          <t>2.6.3</t>
+          <t>2.6.2</t>
         </is>
       </c>
       <c r="F40" s="2" t="inlineStr">
         <is>
-          <t>Piggeries</t>
+          <t>Poultry farms</t>
         </is>
       </c>
     </row>
@@ -1202,12 +1202,12 @@
       <c r="D41" s="2" t="n"/>
       <c r="E41" s="2" t="inlineStr">
         <is>
-          <t>2.6.4</t>
+          <t>2.6.3</t>
         </is>
       </c>
       <c r="F41" s="2" t="inlineStr">
         <is>
-          <t>Horse studs</t>
+          <t>Piggeries</t>
         </is>
       </c>
     </row>
@@ -1218,52 +1218,52 @@
       <c r="D42" s="2" t="n"/>
       <c r="E42" s="2" t="inlineStr">
         <is>
-          <t>2.6.5</t>
+          <t>2.6.4</t>
         </is>
       </c>
       <c r="F42" s="2" t="inlineStr">
         <is>
-          <t>Aquaculture</t>
+          <t>Horse studs</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n"/>
       <c r="B43" s="2" t="n"/>
-      <c r="C43" s="2" t="inlineStr">
-        <is>
-          <t>2.7.0</t>
-        </is>
-      </c>
-      <c r="D43" s="2" t="inlineStr">
-        <is>
-          <t>Water and wastewater</t>
-        </is>
-      </c>
+      <c r="C43" s="2" t="n"/>
+      <c r="D43" s="2" t="n"/>
       <c r="E43" s="2" t="inlineStr">
         <is>
-          <t>2.7.1</t>
+          <t>2.6.5</t>
         </is>
       </c>
       <c r="F43" s="2" t="inlineStr">
         <is>
-          <t>Stock water</t>
+          <t>Aquaculture</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n"/>
       <c r="B44" s="2" t="n"/>
-      <c r="C44" s="2" t="n"/>
-      <c r="D44" s="2" t="n"/>
+      <c r="C44" s="2" t="inlineStr">
+        <is>
+          <t>2.7.0</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>Water and wastewater</t>
+        </is>
+      </c>
       <c r="E44" s="2" t="inlineStr">
         <is>
-          <t>2.7.2</t>
+          <t>2.7.1</t>
         </is>
       </c>
       <c r="F44" s="2" t="inlineStr">
         <is>
-          <t>Effluent pond</t>
+          <t>Stock water</t>
         </is>
       </c>
     </row>
@@ -1274,12 +1274,12 @@
       <c r="D45" s="2" t="n"/>
       <c r="E45" s="2" t="inlineStr">
         <is>
-          <t>2.7.3</t>
+          <t>2.7.2</t>
         </is>
       </c>
       <c r="F45" s="2" t="inlineStr">
         <is>
-          <t>Water treatment – land application</t>
+          <t>Effluent pond</t>
         </is>
       </c>
     </row>
@@ -1290,12 +1290,12 @@
       <c r="D46" s="2" t="n"/>
       <c r="E46" s="2" t="inlineStr">
         <is>
-          <t>2.7.4</t>
+          <t>2.7.3</t>
         </is>
       </c>
       <c r="F46" s="2" t="inlineStr">
         <is>
-          <t>Water treatment – wetland</t>
+          <t>Water treatment – land application</t>
         </is>
       </c>
     </row>
@@ -1306,52 +1306,52 @@
       <c r="D47" s="2" t="n"/>
       <c r="E47" s="2" t="inlineStr">
         <is>
-          <t>2.7.5</t>
+          <t>2.7.4</t>
         </is>
       </c>
       <c r="F47" s="2" t="inlineStr">
         <is>
-          <t>Irrigation reservoirs and canals</t>
+          <t>Water treatment – wetland</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n"/>
       <c r="B48" s="2" t="n"/>
-      <c r="C48" s="2" t="inlineStr">
-        <is>
-          <t>2.8.0</t>
-        </is>
-      </c>
-      <c r="D48" s="2" t="inlineStr">
-        <is>
-          <t>Land in transition</t>
-        </is>
-      </c>
+      <c r="C48" s="2" t="n"/>
+      <c r="D48" s="2" t="n"/>
       <c r="E48" s="2" t="inlineStr">
         <is>
-          <t>2.8.1</t>
+          <t>2.7.5</t>
         </is>
       </c>
       <c r="F48" s="2" t="inlineStr">
         <is>
-          <t>Unused degraded land</t>
+          <t>Irrigation reservoirs and canals</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n"/>
       <c r="B49" s="2" t="n"/>
-      <c r="C49" s="2" t="n"/>
-      <c r="D49" s="2" t="n"/>
+      <c r="C49" s="2" t="inlineStr">
+        <is>
+          <t>2.8.0</t>
+        </is>
+      </c>
+      <c r="D49" s="2" t="inlineStr">
+        <is>
+          <t>Land in transition</t>
+        </is>
+      </c>
       <c r="E49" s="2" t="inlineStr">
         <is>
-          <t>2.8.2</t>
+          <t>2.8.1</t>
         </is>
       </c>
       <c r="F49" s="2" t="inlineStr">
         <is>
-          <t>No defined use</t>
+          <t>Unused degraded land</t>
         </is>
       </c>
     </row>
@@ -1362,12 +1362,12 @@
       <c r="D50" s="2" t="n"/>
       <c r="E50" s="2" t="inlineStr">
         <is>
-          <t>2.8.3</t>
+          <t>2.8.2</t>
         </is>
       </c>
       <c r="F50" s="2" t="inlineStr">
         <is>
-          <t>Land undergoing rehabilitation</t>
+          <t>No defined use</t>
         </is>
       </c>
     </row>
@@ -1378,60 +1378,60 @@
       <c r="D51" s="2" t="n"/>
       <c r="E51" s="2" t="inlineStr">
         <is>
+          <t>2.8.3</t>
+        </is>
+      </c>
+      <c r="F51" s="2" t="inlineStr">
+        <is>
+          <t>Land undergoing rehabilitation</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="n"/>
+      <c r="B52" s="2" t="n"/>
+      <c r="C52" s="2" t="n"/>
+      <c r="D52" s="2" t="n"/>
+      <c r="E52" s="2" t="inlineStr">
+        <is>
           <t>2.8.4</t>
         </is>
       </c>
-      <c r="F51" s="2" t="inlineStr">
+      <c r="F52" s="2" t="inlineStr">
         <is>
           <t>Abandoned land</t>
         </is>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" s="2" t="inlineStr">
+    <row r="53">
+      <c r="A53" s="2" t="inlineStr">
         <is>
           <t>3.0.0</t>
         </is>
       </c>
-      <c r="B52" s="2" t="inlineStr">
+      <c r="B53" s="2" t="inlineStr">
         <is>
           <t>Built environment</t>
         </is>
       </c>
-      <c r="C52" s="2" t="inlineStr">
+      <c r="C53" s="2" t="inlineStr">
         <is>
           <t>3.1.0</t>
         </is>
       </c>
-      <c r="D52" s="2" t="inlineStr">
+      <c r="D53" s="2" t="inlineStr">
         <is>
           <t>Residential</t>
         </is>
       </c>
-      <c r="E52" s="2" t="inlineStr">
+      <c r="E53" s="2" t="inlineStr">
         <is>
           <t>3.1.1</t>
         </is>
       </c>
-      <c r="F52" s="2" t="inlineStr">
+      <c r="F53" s="2" t="inlineStr">
         <is>
           <t>High-density residential</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="2" t="n"/>
-      <c r="B53" s="2" t="n"/>
-      <c r="C53" s="2" t="n"/>
-      <c r="D53" s="2" t="n"/>
-      <c r="E53" s="2" t="inlineStr">
-        <is>
-          <t>3.1.2</t>
-        </is>
-      </c>
-      <c r="F53" s="2" t="inlineStr">
-        <is>
-          <t>Medium-density residential</t>
         </is>
       </c>
     </row>
@@ -1442,12 +1442,12 @@
       <c r="D54" s="2" t="n"/>
       <c r="E54" s="2" t="inlineStr">
         <is>
-          <t>3.1.3</t>
+          <t>3.1.2</t>
         </is>
       </c>
       <c r="F54" s="2" t="inlineStr">
         <is>
-          <t>Low-density residential</t>
+          <t>Medium-density residential</t>
         </is>
       </c>
     </row>
@@ -1458,52 +1458,52 @@
       <c r="D55" s="2" t="n"/>
       <c r="E55" s="2" t="inlineStr">
         <is>
-          <t>3.1.4</t>
+          <t>3.1.3</t>
         </is>
       </c>
       <c r="F55" s="2" t="inlineStr">
         <is>
-          <t>Rural residential</t>
+          <t>Low-density residential</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n"/>
       <c r="B56" s="2" t="n"/>
-      <c r="C56" s="2" t="inlineStr">
-        <is>
-          <t>3.2.0</t>
-        </is>
-      </c>
-      <c r="D56" s="2" t="inlineStr">
-        <is>
-          <t>Public recreation and services</t>
-        </is>
-      </c>
+      <c r="C56" s="2" t="n"/>
+      <c r="D56" s="2" t="n"/>
       <c r="E56" s="2" t="inlineStr">
         <is>
-          <t>3.2.1</t>
+          <t>3.1.4</t>
         </is>
       </c>
       <c r="F56" s="2" t="inlineStr">
         <is>
-          <t>Outdoor recreation</t>
+          <t>Rural residential</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n"/>
       <c r="B57" s="2" t="n"/>
-      <c r="C57" s="2" t="n"/>
-      <c r="D57" s="2" t="n"/>
+      <c r="C57" s="2" t="inlineStr">
+        <is>
+          <t>3.2.0</t>
+        </is>
+      </c>
+      <c r="D57" s="2" t="inlineStr">
+        <is>
+          <t>Public recreation and services</t>
+        </is>
+      </c>
       <c r="E57" s="2" t="inlineStr">
         <is>
-          <t>3.2.2</t>
+          <t>3.2.1</t>
         </is>
       </c>
       <c r="F57" s="2" t="inlineStr">
         <is>
-          <t>Indoor recreation</t>
+          <t>Outdoor recreation</t>
         </is>
       </c>
     </row>
@@ -1514,52 +1514,52 @@
       <c r="D58" s="2" t="n"/>
       <c r="E58" s="2" t="inlineStr">
         <is>
-          <t>3.2.3</t>
+          <t>3.2.2</t>
         </is>
       </c>
       <c r="F58" s="2" t="inlineStr">
         <is>
-          <t>Community services</t>
+          <t>Indoor recreation</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n"/>
       <c r="B59" s="2" t="n"/>
-      <c r="C59" s="2" t="inlineStr">
-        <is>
-          <t>3.3.0</t>
-        </is>
-      </c>
-      <c r="D59" s="2" t="inlineStr">
-        <is>
-          <t>Commercial</t>
-        </is>
-      </c>
+      <c r="C59" s="2" t="n"/>
+      <c r="D59" s="2" t="n"/>
       <c r="E59" s="2" t="inlineStr">
         <is>
-          <t>3.3.1</t>
+          <t>3.2.3</t>
         </is>
       </c>
       <c r="F59" s="2" t="inlineStr">
         <is>
-          <t>Retail</t>
+          <t>Community services</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n"/>
       <c r="B60" s="2" t="n"/>
-      <c r="C60" s="2" t="n"/>
-      <c r="D60" s="2" t="n"/>
+      <c r="C60" s="2" t="inlineStr">
+        <is>
+          <t>3.3.0</t>
+        </is>
+      </c>
+      <c r="D60" s="2" t="inlineStr">
+        <is>
+          <t>Commercial</t>
+        </is>
+      </c>
       <c r="E60" s="2" t="inlineStr">
         <is>
-          <t>3.3.2</t>
+          <t>3.3.1</t>
         </is>
       </c>
       <c r="F60" s="2" t="inlineStr">
         <is>
-          <t>Office</t>
+          <t>Retail</t>
         </is>
       </c>
     </row>
@@ -1570,12 +1570,12 @@
       <c r="D61" s="2" t="n"/>
       <c r="E61" s="2" t="inlineStr">
         <is>
-          <t>3.3.3</t>
+          <t>3.3.2</t>
         </is>
       </c>
       <c r="F61" s="2" t="inlineStr">
         <is>
-          <t>Hospitality</t>
+          <t>Office</t>
         </is>
       </c>
     </row>
@@ -1586,12 +1586,12 @@
       <c r="D62" s="2" t="n"/>
       <c r="E62" s="2" t="inlineStr">
         <is>
-          <t>3.3.4</t>
+          <t>3.3.3</t>
         </is>
       </c>
       <c r="F62" s="2" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Hospitality</t>
         </is>
       </c>
     </row>
@@ -1602,12 +1602,12 @@
       <c r="D63" s="2" t="n"/>
       <c r="E63" s="2" t="inlineStr">
         <is>
-          <t>3.3.5</t>
+          <t>3.3.4</t>
         </is>
       </c>
       <c r="F63" s="2" t="inlineStr">
         <is>
-          <t>Healthcare</t>
+          <t>Entertainment</t>
         </is>
       </c>
     </row>
@@ -1618,52 +1618,52 @@
       <c r="D64" s="2" t="n"/>
       <c r="E64" s="2" t="inlineStr">
         <is>
-          <t>3.3.6</t>
+          <t>3.3.5</t>
         </is>
       </c>
       <c r="F64" s="2" t="inlineStr">
         <is>
-          <t>Transportation &amp; warehousing</t>
+          <t>Healthcare</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n"/>
       <c r="B65" s="2" t="n"/>
-      <c r="C65" s="2" t="inlineStr">
-        <is>
-          <t>3.4.0</t>
-        </is>
-      </c>
-      <c r="D65" s="2" t="inlineStr">
-        <is>
-          <t>Manufacturing and industrial</t>
-        </is>
-      </c>
+      <c r="C65" s="2" t="n"/>
+      <c r="D65" s="2" t="n"/>
       <c r="E65" s="2" t="inlineStr">
         <is>
-          <t>3.4.1</t>
+          <t>3.3.6</t>
         </is>
       </c>
       <c r="F65" s="2" t="inlineStr">
         <is>
-          <t>General purpose factory</t>
+          <t>Transportation &amp; warehousing</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n"/>
       <c r="B66" s="2" t="n"/>
-      <c r="C66" s="2" t="n"/>
-      <c r="D66" s="2" t="n"/>
+      <c r="C66" s="2" t="inlineStr">
+        <is>
+          <t>3.4.0</t>
+        </is>
+      </c>
+      <c r="D66" s="2" t="inlineStr">
+        <is>
+          <t>Manufacturing and industrial</t>
+        </is>
+      </c>
       <c r="E66" s="2" t="inlineStr">
         <is>
-          <t>3.4.2</t>
+          <t>3.4.1</t>
         </is>
       </c>
       <c r="F66" s="2" t="inlineStr">
         <is>
-          <t>Food processing factory</t>
+          <t>General purpose factory</t>
         </is>
       </c>
     </row>
@@ -1674,12 +1674,12 @@
       <c r="D67" s="2" t="n"/>
       <c r="E67" s="2" t="inlineStr">
         <is>
-          <t>3.4.3</t>
+          <t>3.4.2</t>
         </is>
       </c>
       <c r="F67" s="2" t="inlineStr">
         <is>
-          <t>Major industrial complex</t>
+          <t>Food processing factory</t>
         </is>
       </c>
     </row>
@@ -1690,12 +1690,12 @@
       <c r="D68" s="2" t="n"/>
       <c r="E68" s="2" t="inlineStr">
         <is>
-          <t>3.4.4</t>
+          <t>3.4.3</t>
         </is>
       </c>
       <c r="F68" s="2" t="inlineStr">
         <is>
-          <t>Sawmill</t>
+          <t>Major industrial complex</t>
         </is>
       </c>
     </row>
@@ -1706,12 +1706,12 @@
       <c r="D69" s="2" t="n"/>
       <c r="E69" s="2" t="inlineStr">
         <is>
-          <t>3.4.5</t>
+          <t>3.4.4</t>
         </is>
       </c>
       <c r="F69" s="2" t="inlineStr">
         <is>
-          <t>Farm buildings/infrastructure</t>
+          <t>Sawmill</t>
         </is>
       </c>
     </row>
@@ -1722,52 +1722,52 @@
       <c r="D70" s="2" t="n"/>
       <c r="E70" s="2" t="inlineStr">
         <is>
-          <t>3.4.6</t>
+          <t>3.4.5</t>
         </is>
       </c>
       <c r="F70" s="2" t="inlineStr">
         <is>
-          <t>Abattoirs</t>
+          <t>Farm buildings/infrastructure</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n"/>
       <c r="B71" s="2" t="n"/>
-      <c r="C71" s="2" t="inlineStr">
-        <is>
-          <t>3.5.0</t>
-        </is>
-      </c>
-      <c r="D71" s="2" t="inlineStr">
-        <is>
-          <t>Utilities</t>
-        </is>
-      </c>
+      <c r="C71" s="2" t="n"/>
+      <c r="D71" s="2" t="n"/>
       <c r="E71" s="2" t="inlineStr">
         <is>
-          <t>3.5.1</t>
+          <t>3.4.6</t>
         </is>
       </c>
       <c r="F71" s="2" t="inlineStr">
         <is>
-          <t>Fuel powered electricity generation</t>
+          <t>Abattoirs</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n"/>
       <c r="B72" s="2" t="n"/>
-      <c r="C72" s="2" t="n"/>
-      <c r="D72" s="2" t="n"/>
+      <c r="C72" s="2" t="inlineStr">
+        <is>
+          <t>3.5.0</t>
+        </is>
+      </c>
+      <c r="D72" s="2" t="inlineStr">
+        <is>
+          <t>Utilities</t>
+        </is>
+      </c>
       <c r="E72" s="2" t="inlineStr">
         <is>
-          <t>3.5.2</t>
+          <t>3.5.1</t>
         </is>
       </c>
       <c r="F72" s="2" t="inlineStr">
         <is>
-          <t>Hydroelectricity generation</t>
+          <t>Fuel powered electricity generation</t>
         </is>
       </c>
     </row>
@@ -1778,12 +1778,12 @@
       <c r="D73" s="2" t="n"/>
       <c r="E73" s="2" t="inlineStr">
         <is>
-          <t>3.5.3</t>
+          <t>3.5.2</t>
         </is>
       </c>
       <c r="F73" s="2" t="inlineStr">
         <is>
-          <t>Wind electricity generation</t>
+          <t>Hydroelectricity generation</t>
         </is>
       </c>
     </row>
@@ -1794,12 +1794,12 @@
       <c r="D74" s="2" t="n"/>
       <c r="E74" s="2" t="inlineStr">
         <is>
-          <t>3.5.4</t>
+          <t>3.5.3</t>
         </is>
       </c>
       <c r="F74" s="2" t="inlineStr">
         <is>
-          <t>Solar electricity generation</t>
+          <t>Wind electricity generation</t>
         </is>
       </c>
     </row>
@@ -1810,12 +1810,12 @@
       <c r="D75" s="2" t="n"/>
       <c r="E75" s="2" t="inlineStr">
         <is>
-          <t>3.5.5</t>
+          <t>3.5.4</t>
         </is>
       </c>
       <c r="F75" s="2" t="inlineStr">
         <is>
-          <t>Electricity substations and transmission</t>
+          <t>Solar electricity generation</t>
         </is>
       </c>
     </row>
@@ -1826,12 +1826,12 @@
       <c r="D76" s="2" t="n"/>
       <c r="E76" s="2" t="inlineStr">
         <is>
-          <t>3.5.6</t>
+          <t>3.5.5</t>
         </is>
       </c>
       <c r="F76" s="2" t="inlineStr">
         <is>
-          <t>Gas treatment, storage, and transmission</t>
+          <t>Electricity substations and transmission</t>
         </is>
       </c>
     </row>
@@ -1842,52 +1842,52 @@
       <c r="D77" s="2" t="n"/>
       <c r="E77" s="2" t="inlineStr">
         <is>
-          <t>3.5.7</t>
+          <t>3.5.6</t>
         </is>
       </c>
       <c r="F77" s="2" t="inlineStr">
         <is>
-          <t>Water extraction and transmission</t>
+          <t>Gas treatment, storage, and transmission</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n"/>
       <c r="B78" s="2" t="n"/>
-      <c r="C78" s="2" t="inlineStr">
-        <is>
-          <t>3.6.0</t>
-        </is>
-      </c>
-      <c r="D78" s="2" t="inlineStr">
-        <is>
-          <t>Transport and communication</t>
-        </is>
-      </c>
+      <c r="C78" s="2" t="n"/>
+      <c r="D78" s="2" t="n"/>
       <c r="E78" s="2" t="inlineStr">
         <is>
-          <t>3.6.1</t>
+          <t>3.5.7</t>
         </is>
       </c>
       <c r="F78" s="2" t="inlineStr">
         <is>
-          <t>Airports/aerodromes</t>
+          <t>Water extraction and transmission</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n"/>
       <c r="B79" s="2" t="n"/>
-      <c r="C79" s="2" t="n"/>
-      <c r="D79" s="2" t="n"/>
+      <c r="C79" s="2" t="inlineStr">
+        <is>
+          <t>3.6.0</t>
+        </is>
+      </c>
+      <c r="D79" s="2" t="inlineStr">
+        <is>
+          <t>Transport and communication</t>
+        </is>
+      </c>
       <c r="E79" s="2" t="inlineStr">
         <is>
-          <t>3.6.2</t>
+          <t>3.6.1</t>
         </is>
       </c>
       <c r="F79" s="2" t="inlineStr">
         <is>
-          <t>Roads</t>
+          <t>Airports/aerodromes</t>
         </is>
       </c>
     </row>
@@ -1898,12 +1898,12 @@
       <c r="D80" s="2" t="n"/>
       <c r="E80" s="2" t="inlineStr">
         <is>
-          <t>3.6.3</t>
+          <t>3.6.2</t>
         </is>
       </c>
       <c r="F80" s="2" t="inlineStr">
         <is>
-          <t>Railways</t>
+          <t>Roads</t>
         </is>
       </c>
     </row>
@@ -1914,12 +1914,12 @@
       <c r="D81" s="2" t="n"/>
       <c r="E81" s="2" t="inlineStr">
         <is>
-          <t>3.6.4</t>
+          <t>3.6.3</t>
         </is>
       </c>
       <c r="F81" s="2" t="inlineStr">
         <is>
-          <t>Ports and water transport</t>
+          <t>Railways</t>
         </is>
       </c>
     </row>
@@ -1930,52 +1930,52 @@
       <c r="D82" s="2" t="n"/>
       <c r="E82" s="2" t="inlineStr">
         <is>
-          <t>3.6.5</t>
+          <t>3.6.4</t>
         </is>
       </c>
       <c r="F82" s="2" t="inlineStr">
         <is>
-          <t>Navigation and communication</t>
+          <t>Ports and water transport</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="n"/>
       <c r="B83" s="2" t="n"/>
-      <c r="C83" s="2" t="inlineStr">
-        <is>
-          <t>3.7.0</t>
-        </is>
-      </c>
-      <c r="D83" s="2" t="inlineStr">
-        <is>
-          <t>Mining</t>
-        </is>
-      </c>
+      <c r="C83" s="2" t="n"/>
+      <c r="D83" s="2" t="n"/>
       <c r="E83" s="2" t="inlineStr">
         <is>
-          <t>3.7.1</t>
+          <t>3.6.5</t>
         </is>
       </c>
       <c r="F83" s="2" t="inlineStr">
         <is>
-          <t>Mines</t>
+          <t>Navigation and communication</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="n"/>
       <c r="B84" s="2" t="n"/>
-      <c r="C84" s="2" t="n"/>
-      <c r="D84" s="2" t="n"/>
+      <c r="C84" s="2" t="inlineStr">
+        <is>
+          <t>3.7.0</t>
+        </is>
+      </c>
+      <c r="D84" s="2" t="inlineStr">
+        <is>
+          <t>Mining</t>
+        </is>
+      </c>
       <c r="E84" s="2" t="inlineStr">
         <is>
-          <t>3.7.2</t>
+          <t>3.7.1</t>
         </is>
       </c>
       <c r="F84" s="2" t="inlineStr">
         <is>
-          <t>Quarries</t>
+          <t>Mines</t>
         </is>
       </c>
     </row>
@@ -1986,12 +1986,12 @@
       <c r="D85" s="2" t="n"/>
       <c r="E85" s="2" t="inlineStr">
         <is>
-          <t>3.7.3</t>
+          <t>3.7.2</t>
         </is>
       </c>
       <c r="F85" s="2" t="inlineStr">
         <is>
-          <t>Tailings</t>
+          <t>Quarries</t>
         </is>
       </c>
     </row>
@@ -2002,12 +2002,12 @@
       <c r="D86" s="2" t="n"/>
       <c r="E86" s="2" t="inlineStr">
         <is>
-          <t>3.7.4</t>
+          <t>3.7.3</t>
         </is>
       </c>
       <c r="F86" s="2" t="inlineStr">
         <is>
-          <t>Evaporation basins</t>
+          <t>Tailings</t>
         </is>
       </c>
     </row>
@@ -2018,52 +2018,52 @@
       <c r="D87" s="2" t="n"/>
       <c r="E87" s="2" t="inlineStr">
         <is>
-          <t>3.7.5</t>
+          <t>3.7.4</t>
         </is>
       </c>
       <c r="F87" s="2" t="inlineStr">
         <is>
-          <t>Extractive industry not in use</t>
+          <t>Evaporation basins</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="n"/>
       <c r="B88" s="2" t="n"/>
-      <c r="C88" s="2" t="inlineStr">
-        <is>
-          <t>3.8.0</t>
-        </is>
-      </c>
-      <c r="D88" s="2" t="inlineStr">
-        <is>
-          <t>Waste treatment and disposal</t>
-        </is>
-      </c>
+      <c r="C88" s="2" t="n"/>
+      <c r="D88" s="2" t="n"/>
       <c r="E88" s="2" t="inlineStr">
         <is>
-          <t>3.8.1</t>
+          <t>3.7.5</t>
         </is>
       </c>
       <c r="F88" s="2" t="inlineStr">
         <is>
-          <t>Landfills</t>
+          <t>Extractive industry not in use</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="2" t="n"/>
       <c r="B89" s="2" t="n"/>
-      <c r="C89" s="2" t="n"/>
-      <c r="D89" s="2" t="n"/>
+      <c r="C89" s="2" t="inlineStr">
+        <is>
+          <t>3.8.0</t>
+        </is>
+      </c>
+      <c r="D89" s="2" t="inlineStr">
+        <is>
+          <t>Waste treatment and disposal</t>
+        </is>
+      </c>
       <c r="E89" s="2" t="inlineStr">
         <is>
-          <t>3.8.2</t>
+          <t>3.8.1</t>
         </is>
       </c>
       <c r="F89" s="2" t="inlineStr">
         <is>
-          <t>Transfer stations and recycling facilities</t>
+          <t>Landfills</t>
         </is>
       </c>
     </row>
@@ -2074,12 +2074,12 @@
       <c r="D90" s="2" t="n"/>
       <c r="E90" s="2" t="inlineStr">
         <is>
-          <t>3.8.3</t>
+          <t>3.8.2</t>
         </is>
       </c>
       <c r="F90" s="2" t="inlineStr">
         <is>
-          <t>Municipal wastewater</t>
+          <t>Transfer stations and recycling facilities</t>
         </is>
       </c>
     </row>
@@ -2090,12 +2090,12 @@
       <c r="D91" s="2" t="n"/>
       <c r="E91" s="2" t="inlineStr">
         <is>
-          <t>3.8.4</t>
+          <t>3.8.3</t>
         </is>
       </c>
       <c r="F91" s="2" t="inlineStr">
         <is>
-          <t>Wastewater treatment – land application</t>
+          <t>Municipal wastewater</t>
         </is>
       </c>
     </row>
@@ -2106,52 +2106,52 @@
       <c r="D92" s="2" t="n"/>
       <c r="E92" s="2" t="inlineStr">
         <is>
-          <t>3.8.5</t>
+          <t>3.8.4</t>
         </is>
       </c>
       <c r="F92" s="2" t="inlineStr">
         <is>
-          <t>Stormwater management</t>
+          <t>Wastewater treatment – land application</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="n"/>
       <c r="B93" s="2" t="n"/>
-      <c r="C93" s="2" t="inlineStr">
-        <is>
-          <t>3.9.0</t>
-        </is>
-      </c>
-      <c r="D93" s="2" t="inlineStr">
-        <is>
-          <t>Vacant and transitioning land</t>
-        </is>
-      </c>
+      <c r="C93" s="2" t="n"/>
+      <c r="D93" s="2" t="n"/>
       <c r="E93" s="2" t="inlineStr">
         <is>
-          <t>3.9.1</t>
+          <t>3.8.5</t>
         </is>
       </c>
       <c r="F93" s="2" t="inlineStr">
         <is>
-          <t>Vacant land</t>
+          <t>Stormwater management</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="n"/>
       <c r="B94" s="2" t="n"/>
-      <c r="C94" s="2" t="n"/>
-      <c r="D94" s="2" t="n"/>
+      <c r="C94" s="2" t="inlineStr">
+        <is>
+          <t>3.9.0</t>
+        </is>
+      </c>
+      <c r="D94" s="2" t="inlineStr">
+        <is>
+          <t>Vacant and transitioning land</t>
+        </is>
+      </c>
       <c r="E94" s="2" t="inlineStr">
         <is>
-          <t>3.9.2</t>
+          <t>3.9.1</t>
         </is>
       </c>
       <c r="F94" s="2" t="inlineStr">
         <is>
-          <t>Greenfield development</t>
+          <t>Vacant land</t>
         </is>
       </c>
     </row>
@@ -2162,10 +2162,26 @@
       <c r="D95" s="2" t="n"/>
       <c r="E95" s="2" t="inlineStr">
         <is>
+          <t>3.9.2</t>
+        </is>
+      </c>
+      <c r="F95" s="2" t="inlineStr">
+        <is>
+          <t>Greenfield development</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="n"/>
+      <c r="B96" s="2" t="n"/>
+      <c r="C96" s="2" t="n"/>
+      <c r="D96" s="2" t="n"/>
+      <c r="E96" s="2" t="inlineStr">
+        <is>
           <t>3.9.3</t>
         </is>
       </c>
-      <c r="F95" s="2" t="inlineStr">
+      <c r="F96" s="2" t="inlineStr">
         <is>
           <t>Brownfield development</t>
         </is>
@@ -2173,54 +2189,54 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="C71:C77"/>
-    <mergeCell ref="B52:B95"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C57:C59"/>
+    <mergeCell ref="D60:D65"/>
     <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C43:C47"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="D72:D78"/>
     <mergeCell ref="C2:C8"/>
-    <mergeCell ref="D93:D95"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D59:D64"/>
-    <mergeCell ref="B22:B51"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="D49:D52"/>
+    <mergeCell ref="C39:C43"/>
     <mergeCell ref="D9:D11"/>
-    <mergeCell ref="D43:D47"/>
-    <mergeCell ref="D65:D70"/>
-    <mergeCell ref="D71:D77"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="D83:D87"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="D39:D43"/>
     <mergeCell ref="A2:A21"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="C38:C42"/>
-    <mergeCell ref="C65:C70"/>
-    <mergeCell ref="D38:D42"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C59:C64"/>
-    <mergeCell ref="D88:D92"/>
-    <mergeCell ref="C78:C82"/>
-    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="D79:D83"/>
+    <mergeCell ref="C72:C78"/>
+    <mergeCell ref="D89:D93"/>
+    <mergeCell ref="D94:D96"/>
+    <mergeCell ref="B53:B96"/>
+    <mergeCell ref="A22:A52"/>
+    <mergeCell ref="D44:D48"/>
+    <mergeCell ref="D66:D71"/>
+    <mergeCell ref="D22:D26"/>
+    <mergeCell ref="D84:D88"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="A53:A96"/>
     <mergeCell ref="C12:C19"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C89:C93"/>
+    <mergeCell ref="C94:C96"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="D53:D56"/>
     <mergeCell ref="D20:D21"/>
-    <mergeCell ref="C83:C87"/>
-    <mergeCell ref="C93:C95"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="C88:C92"/>
-    <mergeCell ref="A52:A95"/>
-    <mergeCell ref="A22:A51"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="C79:C83"/>
+    <mergeCell ref="B22:B52"/>
+    <mergeCell ref="C44:C48"/>
+    <mergeCell ref="C60:C65"/>
+    <mergeCell ref="C66:C71"/>
     <mergeCell ref="D12:D19"/>
-    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="D57:D59"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C84:C88"/>
     <mergeCell ref="D2:D8"/>
+    <mergeCell ref="C53:C56"/>
     <mergeCell ref="B2:B21"/>
-    <mergeCell ref="D78:D82"/>
     <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C49:C52"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>